<commit_message>
added L3 to course Mapp
</commit_message>
<xml_diff>
--- a/docs/Comp_Module_Map_2022_V5.xlsx
+++ b/docs/Comp_Module_Map_2022_V5.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ssu-my.sharepoint.com/personal/martin_reid_solent_ac_uk/Documents/comp_course_manage_2020/comp_planning_2021-22/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ssu-my.sharepoint.com/personal/martin_reid_solent_ac_uk/Documents/solent_store/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="8_{F910275D-011D-4B9B-94BD-9ED687CDE8E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A91724BA-580F-46FC-AE1E-7BBE67F00D04}"/>
+  <xr:revisionPtr revIDLastSave="82" documentId="8_{F910275D-011D-4B9B-94BD-9ED687CDE8E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{62DFF729-FD9A-8947-8F76-0EBE44DF1880}"/>
   <bookViews>
-    <workbookView xWindow="-27870" yWindow="3090" windowWidth="24015" windowHeight="14400" xr2:uid="{E69C05BD-5864-2041-BCC3-203BAAF63D0E}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="28340" activeTab="3" xr2:uid="{E69C05BD-5864-2041-BCC3-203BAAF63D0E}"/>
   </bookViews>
   <sheets>
-    <sheet name="UG Map" sheetId="1" r:id="rId1"/>
-    <sheet name="PG Map" sheetId="5" r:id="rId2"/>
-    <sheet name="PG MAIDS" sheetId="3" r:id="rId3"/>
+    <sheet name="Foundation" sheetId="6" r:id="rId1"/>
+    <sheet name="UG Map L4-L6" sheetId="1" r:id="rId2"/>
+    <sheet name="PG Map" sheetId="5" r:id="rId3"/>
+    <sheet name="PG MAIDS" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="99">
   <si>
     <t>COM411 Problem Solving Through Programming</t>
   </si>
@@ -335,6 +336,27 @@
   </si>
   <si>
     <t>COM427 Principles and Methods of Data Analysis  (Apprentice only module) Kenton (AL)</t>
+  </si>
+  <si>
+    <t>Computing Foundation</t>
+  </si>
+  <si>
+    <t>COM306 Digital Media Technologies</t>
+  </si>
+  <si>
+    <t>COM300 Problem Solving</t>
+  </si>
+  <si>
+    <t>COM302 Group Technology Project</t>
+  </si>
+  <si>
+    <t>COM304 Foundation Computing</t>
+  </si>
+  <si>
+    <t>COM305 Induviudual Degree Related Project</t>
+  </si>
+  <si>
+    <t>COM307 Foundation Mathematics</t>
   </si>
 </sst>
 </file>
@@ -773,7 +795,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -948,6 +970,22 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1263,23 +1301,103 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F30BF1D-852F-3C41-AD35-7CF114F6F6A5}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6.5" customWidth="1"/>
+    <col min="2" max="2" width="41" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="76" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="77"/>
+    </row>
+    <row r="2" spans="1:2" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="78"/>
+      <c r="B2" s="79"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="18">
+        <v>1</v>
+      </c>
+      <c r="B3" s="75" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="16">
+        <v>2</v>
+      </c>
+      <c r="B4" s="39" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="18">
+        <v>3</v>
+      </c>
+      <c r="B5" s="75" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="16">
+        <v>4</v>
+      </c>
+      <c r="B6" s="39" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="18">
+        <v>5</v>
+      </c>
+      <c r="B7" s="75" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="74">
+        <v>6</v>
+      </c>
+      <c r="B8" s="42" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFDE26D5-4215-1D47-A0E4-BF6B097FFA25}">
   <dimension ref="A1:I55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.125" customWidth="1"/>
+    <col min="1" max="1" width="6.1640625" customWidth="1"/>
     <col min="2" max="2" width="76.5" customWidth="1"/>
-    <col min="7" max="7" width="11.625" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" customWidth="1"/>
     <col min="8" max="8" width="13.5" customWidth="1"/>
-    <col min="9" max="9" width="12.25" customWidth="1"/>
+    <col min="9" max="9" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="26.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="26" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="60" t="s">
         <v>59</v>
       </c>
@@ -1296,7 +1414,7 @@
       </c>
       <c r="I1" s="67"/>
     </row>
-    <row r="2" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="62"/>
       <c r="B2" s="62"/>
       <c r="C2" s="47" t="s">
@@ -1321,7 +1439,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="12">
         <v>1</v>
       </c>
@@ -1350,7 +1468,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="16">
         <v>2</v>
       </c>
@@ -1377,7 +1495,7 @@
       </c>
       <c r="I4" s="17"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="18">
         <v>3</v>
       </c>
@@ -1396,7 +1514,7 @@
       <c r="H5" s="6"/>
       <c r="I5" s="19"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="16">
         <v>4</v>
       </c>
@@ -1417,7 +1535,7 @@
       </c>
       <c r="I6" s="17"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="18">
         <v>5</v>
       </c>
@@ -1438,7 +1556,7 @@
       </c>
       <c r="I7" s="19"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="16">
         <v>6</v>
       </c>
@@ -1457,7 +1575,7 @@
       <c r="H8" s="2"/>
       <c r="I8" s="17"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="18">
         <v>7</v>
       </c>
@@ -1486,7 +1604,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="16">
         <v>8</v>
       </c>
@@ -1507,7 +1625,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="18">
         <v>9</v>
       </c>
@@ -1528,7 +1646,7 @@
       <c r="H11" s="6"/>
       <c r="I11" s="19"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="16">
         <v>10</v>
       </c>
@@ -1545,7 +1663,7 @@
       <c r="H12" s="2"/>
       <c r="I12" s="20"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="18">
         <v>11</v>
       </c>
@@ -1564,7 +1682,7 @@
       </c>
       <c r="I13" s="19"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="16">
         <v>12</v>
       </c>
@@ -1581,7 +1699,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="18">
         <v>13</v>
       </c>
@@ -1600,7 +1718,7 @@
       </c>
       <c r="I15" s="20"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="18">
         <v>15</v>
       </c>
@@ -1617,7 +1735,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="51">
         <v>16</v>
       </c>
@@ -1636,7 +1754,7 @@
       </c>
       <c r="I17" s="69"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="12">
         <v>17</v>
       </c>
@@ -1657,7 +1775,7 @@
       </c>
       <c r="I18" s="41"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="22">
         <v>18</v>
       </c>
@@ -1676,7 +1794,7 @@
       </c>
       <c r="I19" s="40"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="18">
         <v>19</v>
       </c>
@@ -1701,7 +1819,7 @@
       <c r="H20" s="35"/>
       <c r="I20" s="40"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="22">
         <v>20</v>
       </c>
@@ -1720,7 +1838,7 @@
       </c>
       <c r="I21" s="40"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="18">
         <v>21</v>
       </c>
@@ -1739,7 +1857,7 @@
       <c r="H22" s="35"/>
       <c r="I22" s="40"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="22">
         <v>22</v>
       </c>
@@ -1758,7 +1876,7 @@
       </c>
       <c r="I23" s="40"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="18">
         <v>23</v>
       </c>
@@ -1781,7 +1899,7 @@
       </c>
       <c r="I24" s="40"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="22">
         <v>24</v>
       </c>
@@ -1802,7 +1920,7 @@
       </c>
       <c r="I25" s="40"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="18">
         <v>25</v>
       </c>
@@ -1823,7 +1941,7 @@
       </c>
       <c r="I26" s="40"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="22">
         <v>26</v>
       </c>
@@ -1842,7 +1960,7 @@
       </c>
       <c r="I27" s="40"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="18">
         <v>27</v>
       </c>
@@ -1861,7 +1979,7 @@
       </c>
       <c r="I28" s="40"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="22">
         <v>28</v>
       </c>
@@ -1878,7 +1996,7 @@
       <c r="H29" s="36"/>
       <c r="I29" s="40"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="18">
         <v>29</v>
       </c>
@@ -1895,7 +2013,7 @@
       <c r="H30" s="36"/>
       <c r="I30" s="20"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="22">
         <v>30</v>
       </c>
@@ -1912,7 +2030,7 @@
       <c r="H31" s="36"/>
       <c r="I31" s="39"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="18">
         <v>31</v>
       </c>
@@ -1931,7 +2049,7 @@
       </c>
       <c r="I32" s="39"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="22">
         <v>32</v>
       </c>
@@ -1950,7 +2068,7 @@
       </c>
       <c r="I33" s="39"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="18">
         <v>33</v>
       </c>
@@ -1971,7 +2089,7 @@
       </c>
       <c r="I34" s="39"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="22">
         <v>34</v>
       </c>
@@ -1988,7 +2106,7 @@
       </c>
       <c r="I35" s="39"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="18">
         <v>35</v>
       </c>
@@ -2005,7 +2123,7 @@
       </c>
       <c r="I36" s="39"/>
     </row>
-    <row r="37" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="23">
         <v>36</v>
       </c>
@@ -2022,7 +2140,7 @@
       </c>
       <c r="I37" s="42"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="12">
         <v>37</v>
       </c>
@@ -2043,7 +2161,7 @@
       <c r="H38" s="14"/>
       <c r="I38" s="38"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="22">
         <v>38</v>
       </c>
@@ -2064,7 +2182,7 @@
       </c>
       <c r="I39" s="39"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="18">
         <v>39</v>
       </c>
@@ -2085,7 +2203,7 @@
       </c>
       <c r="I40" s="39"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="22">
         <v>40</v>
       </c>
@@ -2106,7 +2224,7 @@
       </c>
       <c r="I41" s="39"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="18">
         <v>41</v>
       </c>
@@ -2131,7 +2249,7 @@
       <c r="H42" s="6"/>
       <c r="I42" s="39"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="22">
         <v>42</v>
       </c>
@@ -2158,7 +2276,7 @@
       </c>
       <c r="I43" s="39"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="18">
         <v>43</v>
       </c>
@@ -2181,7 +2299,7 @@
       </c>
       <c r="I44" s="39"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="22">
         <v>44</v>
       </c>
@@ -2202,7 +2320,7 @@
       </c>
       <c r="I45" s="39"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="18">
         <v>45</v>
       </c>
@@ -2223,7 +2341,7 @@
       <c r="H46" s="6"/>
       <c r="I46" s="39"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="22">
         <v>46</v>
       </c>
@@ -2238,7 +2356,7 @@
       <c r="H47" s="4"/>
       <c r="I47" s="39"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="18">
         <v>47</v>
       </c>
@@ -2255,7 +2373,7 @@
       <c r="H48" s="6"/>
       <c r="I48" s="39"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="22">
         <v>48</v>
       </c>
@@ -2276,7 +2394,7 @@
       </c>
       <c r="I49" s="39"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="18">
         <v>49</v>
       </c>
@@ -2295,7 +2413,7 @@
       </c>
       <c r="I50" s="39"/>
     </row>
-    <row r="51" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="23">
         <v>50</v>
       </c>
@@ -2312,10 +2430,10 @@
       </c>
       <c r="I51" s="42"/>
     </row>
-    <row r="52" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="10"/>
     </row>
-    <row r="53" spans="1:9" ht="56.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" ht="56" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A53" s="10"/>
       <c r="B53" s="58" t="s">
         <v>88</v>
@@ -2329,7 +2447,7 @@
       <c r="G53" s="64"/>
       <c r="H53" s="65"/>
     </row>
-    <row r="54" spans="1:9" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="5"/>
       <c r="C54" s="26"/>
       <c r="D54" s="25"/>
@@ -2338,7 +2456,7 @@
       <c r="G54" s="25"/>
       <c r="H54" s="25"/>
     </row>
-    <row r="55" spans="1:9" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C55" s="52"/>
       <c r="D55" s="63" t="s">
         <v>78</v>
@@ -2362,25 +2480,25 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F81969C-1129-7B49-AAFA-87F4D4FA5C16}">
   <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.125" customWidth="1"/>
-    <col min="2" max="2" width="41.625" customWidth="1"/>
-    <col min="3" max="3" width="13.625" customWidth="1"/>
+    <col min="1" max="1" width="6.1640625" customWidth="1"/>
+    <col min="2" max="2" width="41.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
     <col min="4" max="4" width="12.5" customWidth="1"/>
-    <col min="5" max="5" width="11.875" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" customWidth="1"/>
     <col min="6" max="6" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="60" t="s">
         <v>60</v>
       </c>
@@ -2391,7 +2509,7 @@
       <c r="D1" s="71"/>
       <c r="E1" s="72"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="62"/>
       <c r="B2" s="61"/>
       <c r="C2" s="11" t="s">
@@ -2404,7 +2522,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="31">
         <v>1</v>
       </c>
@@ -2421,7 +2539,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="28">
         <v>2</v>
       </c>
@@ -2438,7 +2556,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="31">
         <v>3</v>
       </c>
@@ -2455,7 +2573,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="28">
         <v>4</v>
       </c>
@@ -2468,7 +2586,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="31">
         <v>5</v>
       </c>
@@ -2483,7 +2601,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="28">
         <v>6</v>
       </c>
@@ -2498,7 +2616,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="31">
         <v>7</v>
       </c>
@@ -2512,7 +2630,7 @@
       </c>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="28">
         <v>8</v>
       </c>
@@ -2526,7 +2644,7 @@
       <c r="E10" s="2"/>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="31">
         <v>9</v>
       </c>
@@ -2540,7 +2658,7 @@
       <c r="E11" s="6"/>
       <c r="F11" s="29"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="28">
         <v>10</v>
       </c>
@@ -2554,7 +2672,7 @@
       <c r="E12" s="2"/>
       <c r="F12" s="30"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="31">
         <v>11</v>
       </c>
@@ -2568,7 +2686,7 @@
       <c r="E13" s="6"/>
       <c r="F13" s="30"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="28">
         <v>12</v>
       </c>
@@ -2582,7 +2700,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="30"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="31">
         <v>13</v>
       </c>
@@ -2596,7 +2714,7 @@
       <c r="E15" s="6"/>
       <c r="F15" s="30"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="33">
         <v>14</v>
       </c>
@@ -2614,7 +2732,7 @@
       </c>
       <c r="F16" s="30"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="31">
         <v>15</v>
       </c>
@@ -2632,7 +2750,7 @@
       </c>
       <c r="F17" s="30"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="33">
         <v>16</v>
       </c>
@@ -2650,43 +2768,43 @@
       </c>
       <c r="F18" s="30"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="30"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="30"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="30"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="30"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="30"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="30"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="30"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="30"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="30"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="30"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="29"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="10"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="5"/>
       <c r="C52" s="26"/>
       <c r="D52" s="25"/>
@@ -2701,32 +2819,32 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCA73B5C-D9F3-8C4C-8480-D7DAE5FA9C24}">
   <dimension ref="A1:B52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.125" customWidth="1"/>
-    <col min="2" max="2" width="77.375" customWidth="1"/>
+    <col min="1" max="1" width="6.1640625" customWidth="1"/>
+    <col min="2" max="2" width="77.33203125" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="73" t="s">
         <v>75</v>
       </c>
       <c r="B1" s="73"/>
     </row>
-    <row r="2" spans="1:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="73"/>
       <c r="B2" s="73"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="31">
         <v>1</v>
       </c>
@@ -2734,7 +2852,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="28">
         <v>2</v>
       </c>
@@ -2742,7 +2860,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="31">
         <v>3</v>
       </c>
@@ -2750,7 +2868,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="28">
         <v>4</v>
       </c>
@@ -2758,7 +2876,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="31">
         <v>5</v>
       </c>
@@ -2766,43 +2884,43 @@
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="30"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="30"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" s="30"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" s="30"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" s="30"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" s="30"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" s="30"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" s="30"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" s="30"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" s="30"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" s="29"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" s="10"/>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" s="5"/>
     </row>
   </sheetData>

</xml_diff>